<commit_message>
update test case to include a tie-break
</commit_message>
<xml_diff>
--- a/src/test/resources/network/brightspots/rcv/test_data/test_set_allow_only_one_winner_per_round/test_set_allow_only_one_winner_per_round_cvr.xlsx
+++ b/src/test/resources/network/brightspots/rcv/test_data/test_set_allow_only_one_winner_per_round/test_set_allow_only_one_winner_per_round_cvr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leisenberg/code/rcv/src/test/resources/network/brightspots/rcv/test_data/test_set_only_one_winner_per_round/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leisenberg/code/rcv/src/test/resources/network/brightspots/rcv/test_data/test_set_allow_only_one_winner_per_round/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A79EA66-9DC6-8843-9DE7-253D165A4F3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F373B42-9C74-1C49-A989-DEF2A452F20F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="1180" windowWidth="25280" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
   <si>
     <t>Ballot #</t>
   </si>
@@ -369,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -441,13 +441,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -483,13 +483,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -517,20 +517,6 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>